<commit_message>
Update 1.6.1: Added Remaining Material Analysis Report
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Прогресс Проекта.xlsx
+++ b/pkg/excels/templates/Прогресс Проекта.xlsx
@@ -892,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,336 +961,6 @@
       </c>
       <c r="O1" s="5" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F2" s="4">
-        <f>D2-E2</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
-        <f>E2-G2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F3" s="4">
-        <f t="shared" ref="F2:F34" si="0">D3-E3</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="4">
-        <f t="shared" ref="H3:H34" si="1">E3-G3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F4" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F8" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F18" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F24" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F25" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F26" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F28" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F29" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F30" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F32" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F33" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F34" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H34" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 1.6.2: Added missing Operation part in Project Progress Report
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Прогресс Проекта.xlsx
+++ b/pkg/excels/templates/Прогресс Проекта.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="28800" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Материалы" sheetId="1" r:id="rId1"/>
-    <sheet name="Услуги " sheetId="3" r:id="rId2"/>
+    <sheet name="Услуги" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -302,7 +302,7 @@
     <author>Shavkat-PC</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -330,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -365,33 +365,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Shavkat-PC:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+кол-во выполненно умноженное на цену еденицы услуги с заказчиком</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Shavkat-PC:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-кол-во выполненно умноженное на цену еденицы услуги с заказчиком</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -422,7 +422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Код материала</t>
   </si>
@@ -466,15 +466,6 @@
     <t>Выполнено</t>
   </si>
   <si>
-    <t>В ожидании выполнении</t>
-  </si>
-  <si>
-    <t>Сумма выполнении</t>
-  </si>
-  <si>
-    <t>Сумма в ожидании выполнении</t>
-  </si>
-  <si>
     <t>Запланированный бюджет</t>
   </si>
   <si>
@@ -487,10 +478,16 @@
     <t>Сумма материалов в ожидании установки</t>
   </si>
   <si>
-    <t>Добавить чекбокс для услуги что бы появились в список услуг</t>
-  </si>
-  <si>
     <t>По плану</t>
+  </si>
+  <si>
+    <t>Сумма выполнения</t>
+  </si>
+  <si>
+    <t>Сумма в ожидании выполнения</t>
+  </si>
+  <si>
+    <t>В ожидании выполнения</t>
   </si>
 </sst>
 </file>
@@ -894,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +900,7 @@
     <col min="1" max="1" width="10.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="46.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="2"/>
-    <col min="4" max="4" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="2" customWidth="1"/>
@@ -912,7 +909,7 @@
     <col min="10" max="10" width="13.140625" style="2" customWidth="1"/>
     <col min="11" max="12" width="11" style="2" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="2" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -951,16 +948,16 @@
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -971,25 +968,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N11:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="46.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="2"/>
-    <col min="4" max="4" width="10" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -997,224 +993,23 @@
         <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F2" s="4">
-        <f>D2-E2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F3" s="4">
-        <f t="shared" ref="F3:F34" si="0">D3-E3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F4" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F8" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update 1.6.3: Added new parameter for Project Progress
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Прогресс Проекта.xlsx
+++ b/pkg/excels/templates/Прогресс Проекта.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="28800" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Материалы" sheetId="1" r:id="rId1"/>
@@ -86,32 +86,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Shavkat-PC:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-расход материалов с бригадира на объект - онлайн</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -185,32 +159,6 @@
           </rPr>
           <t xml:space="preserve">
 на объекте расход выполнен но не списан - онлайн</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Shavkat-PC:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-запланированое кол-во умноженная на стоимость с заказчиком</t>
         </r>
       </text>
     </comment>
@@ -466,9 +414,6 @@
     <t>Выполнено</t>
   </si>
   <si>
-    <t>Запланированный бюджет</t>
-  </si>
-  <si>
     <t xml:space="preserve">Сумма полученных материалов </t>
   </si>
   <si>
@@ -488,6 +433,9 @@
   </si>
   <si>
     <t>В ожидании выполнения</t>
+  </si>
+  <si>
+    <t>Списано</t>
   </si>
 </sst>
 </file>
@@ -891,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,22 +895,23 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -970,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N11:N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,19 +942,19 @@
         <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>